<commit_message>
separated data elements with comma for each functionality
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
+++ b/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14955" windowHeight="4140"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>User</t>
   </si>
@@ -38,7 +38,7 @@
     <t>['Verify PIN', 'Deposit Cheque']</t>
   </si>
   <si>
-    <t>,['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type'],['Amt_avail', 'Acc_type']</t>
+    <t>['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']['Amt_avail', 'Acc_type']</t>
   </si>
   <si>
     <t xml:space="preserve"> withdraw cash</t>
@@ -47,7 +47,7 @@
     <t>['Withdraw cash', 'Verify PIN']</t>
   </si>
   <si>
-    <t>,['Bill_type', 'Max_limit'],['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>['Bill_type', 'Max_limit']['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
   </si>
   <si>
     <t xml:space="preserve"> transfer money</t>
@@ -56,7 +56,7 @@
     <t>['Transfer Money', 'Verify PIN']</t>
   </si>
   <si>
-    <t>,['From_AcctNum', 'To_AcctNum', 'Amt_avail', 'Amt_trnsfr'],['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>['From_AcctNum', 'To_AcctNum', 'Amt_avail', 'Amt_trnsfr']['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
   </si>
   <si>
     <t xml:space="preserve"> pay my utility bills</t>
@@ -65,7 +65,7 @@
     <t>['Pay Bills ', 'Withdraw cash']</t>
   </si>
   <si>
-    <t>,['Cus_Nme', 'Amt_avail', 'Acc_type'],['Bill_type', 'Max_limit']</t>
+    <t>['Cus_Nme', 'Amt_avail', 'Acc_type']['Bill_type', 'Max_limit']</t>
   </si>
   <si>
     <t xml:space="preserve"> apply for a loan</t>
@@ -74,7 +74,7 @@
     <t>['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>,['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr'],['Loan_Amt', 'Cred_Score']</t>
+    <t>['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr']['Loan_Amt', 'Cred_Score']</t>
   </si>
   <si>
     <t>Banker</t>
@@ -86,7 +86,7 @@
     <t>['Cheque Services', 'Verify PIN']</t>
   </si>
   <si>
-    <t>,[],['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>[]['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
   </si>
   <si>
     <t xml:space="preserve"> restock sufficient cash</t>
@@ -95,7 +95,7 @@
     <t>['Limit Cash', 'Withdraw cash']</t>
   </si>
   <si>
-    <t>,['Cus_Nme', 'Acc_type'],['Bill_type', 'Max_limit']</t>
+    <t>['Cus_Nme', 'Acc_type']['Bill_type', 'Max_limit']</t>
   </si>
   <si>
     <t xml:space="preserve"> limit the cash withdrawl</t>
@@ -107,7 +107,7 @@
     <t>['Review transactions', 'View Account ']</t>
   </si>
   <si>
-    <t>,[],['Amt_avail']</t>
+    <t>[]['Amt_avail']</t>
   </si>
   <si>
     <t xml:space="preserve"> review the credit history, apply for loans</t>
@@ -116,7 +116,7 @@
     <t>['Credit_check', 'Review transactions'],['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>,['Loan_Amt', 'Cred_Score'],[],,['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr'],['Loan_Amt', 'Cred_Score']</t>
+    <t>['Loan_Amt', 'Cred_Score'][],['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr']['Loan_Amt', 'Cred_Score']</t>
   </si>
   <si>
     <t xml:space="preserve"> operate locker</t>
@@ -128,23 +128,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -159,26 +160,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -466,18 +481,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -643,9 +656,8 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replaced set_value and get_value with at function
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
+++ b/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14955" windowHeight="4140"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>User</t>
   </si>
@@ -134,24 +134,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -166,40 +165,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -487,15 +472,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="47" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -661,8 +649,9 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
+      <c r="D12" t="s"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
checking similarity for each action(keywords) instead of whole keywords or sentence
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
+++ b/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14955" windowHeight="4140"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>User</t>
   </si>
@@ -38,7 +38,7 @@
     <t>['Verify PIN', 'Deposit Cheque']</t>
   </si>
   <si>
-    <t>['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']['Amt_avail', 'Acc_type']</t>
+    <t>{'Cust_Addr', 'Loan_Amt', 'Acc_num', 'Cus_Nme'}{'To_AcctNum', 'Debit_pin', 'Amt_avail', 'Acc_num', 'From_AcctNum'}</t>
   </si>
   <si>
     <t xml:space="preserve"> withdraw cash</t>
@@ -47,7 +47,7 @@
     <t>['Withdraw cash', 'Verify PIN']</t>
   </si>
   <si>
-    <t>['Bill_type', 'Max_limit']['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>{'Debit_pin', 'Max_limit', 'Acc_num', 'Cus_Nme', 'Bill_type'}{'Cust_Addr', 'Loan_Amt', 'Acc_num', 'Cus_Nme'}</t>
   </si>
   <si>
     <t xml:space="preserve"> transfer money</t>
@@ -56,16 +56,16 @@
     <t>['Transfer Money', 'Verify PIN']</t>
   </si>
   <si>
-    <t>['From_AcctNum', 'To_AcctNum', 'Amt_avail', 'Amt_trnsfr']['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>{'Amt_trnsfr', 'To_AcctNum', 'Amt_avail', 'Cus_Nme', 'From_AcctNum'}{'Cust_Addr', 'Loan_Amt', 'Acc_num', 'Cus_Nme'}</t>
   </si>
   <si>
     <t xml:space="preserve"> pay my utility bills</t>
   </si>
   <si>
-    <t>['Pay Bills ', 'Withdraw cash']</t>
-  </si>
-  <si>
-    <t>['Cus_Nme', 'Amt_avail', 'Acc_type']['Bill_type', 'Max_limit']</t>
+    <t>['Pay Bills ']</t>
+  </si>
+  <si>
+    <t>{'Debit_pin', 'Amt_avail', 'Acc_num', 'Bill_type', 'From_AcctNum'}</t>
   </si>
   <si>
     <t xml:space="preserve"> apply for a loan</t>
@@ -74,7 +74,7 @@
     <t>['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr']['Loan_Amt', 'Cred_Score']</t>
+    <t>{'Debit_pin', 'To_AcctNum', 'Acc_num', 'Cus_Nme', 'From_AcctNum'}{'Cred_Score', 'Loan_Amt', 'Loan_purp'}</t>
   </si>
   <si>
     <t>Banker</t>
@@ -83,10 +83,10 @@
     <t xml:space="preserve"> request for check books</t>
   </si>
   <si>
-    <t>['Cheque Services', 'Verify PIN']</t>
-  </si>
-  <si>
-    <t>[]['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>['Cheque Services']</t>
+  </si>
+  <si>
+    <t>{'Cust_Addr', 'Loan_Amt', 'Acc_num', 'Cus_Nme'}</t>
   </si>
   <si>
     <t xml:space="preserve"> restock sufficient cash</t>
@@ -95,16 +95,16 @@
     <t>['Restock cash', 'Limit Cash']</t>
   </si>
   <si>
-    <t>['Cus_Nme', 'Acc_type']['Cus_Nme', 'Acc_type']</t>
+    <t>{'Acc_type', 'Max_limit', 'Acc_num', 'Cus_Nme'}{'Acc_type', 'Debit_pin', 'Amt_deposit', 'Acc_num', 'Cus_Nme'}</t>
   </si>
   <si>
     <t xml:space="preserve"> limit the cash withdrawl</t>
   </si>
   <si>
-    <t>['Limit Cash', 'Withdraw cash']</t>
-  </si>
-  <si>
-    <t>['Cus_Nme', 'Acc_type']['Bill_type', 'Max_limit']</t>
+    <t>['Limit Cash']</t>
+  </si>
+  <si>
+    <t>{'Acc_type', 'Debit_pin', 'Amt_deposit', 'Acc_num', 'Cus_Nme'}</t>
   </si>
   <si>
     <t xml:space="preserve"> review all transactions</t>
@@ -113,7 +113,7 @@
     <t>['Review transactions', 'View Account ']</t>
   </si>
   <si>
-    <t>['Acc_num']['Acc_num', 'Amt_avail']</t>
+    <t>{'Acc_num'}{'Cust_Addr', 'Loan_Amt', 'Acc_num', 'Cus_Nme'}</t>
   </si>
   <si>
     <t xml:space="preserve"> review the credit history, apply for loans</t>
@@ -122,7 +122,7 @@
     <t>['Credit_check', 'Review transactions'],['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>['Loan_Amt', 'Cred_Score']['Acc_num'],['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr']['Loan_Amt', 'Cred_Score']</t>
+    <t>{'Cred_Score', 'Loan_Amt', 'Loan_purp'}{'Acc_num'},{'Debit_pin', 'To_AcctNum', 'Acc_num', 'Cus_Nme', 'From_AcctNum'}{'Cred_Score', 'Loan_Amt', 'Loan_purp'}</t>
   </si>
   <si>
     <t xml:space="preserve"> operate locker</t>
@@ -134,23 +134,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -165,26 +166,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,18 +487,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="89.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -649,9 +664,8 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
checking similarity aganist each action(keyword) instead of comparing whole keywords
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
+++ b/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="10545" windowHeight="3585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>User</t>
   </si>
@@ -38,7 +38,7 @@
     <t>['Verify PIN', 'Deposit Cheque']</t>
   </si>
   <si>
-    <t>['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']['Amt_avail', 'Acc_type']</t>
+    <t>{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}{'Debit_pin', 'Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> withdraw cash</t>
@@ -47,7 +47,7 @@
     <t>['Withdraw cash', 'Verify PIN']</t>
   </si>
   <si>
-    <t>['Bill_type', 'Max_limit']['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>{'Debit_pin', 'Bill_type', 'Max_limit', 'Cus_Nme', 'Acc_num'}{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> transfer money</t>
@@ -56,16 +56,16 @@
     <t>['Transfer Money', 'Verify PIN']</t>
   </si>
   <si>
-    <t>['From_AcctNum', 'To_AcctNum', 'Amt_avail', 'Amt_trnsfr']['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>{'Amt_trnsfr', 'Amt_avail', 'Cus_Nme', 'To_AcctNum', 'From_AcctNum'}{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> pay my utility bills</t>
   </si>
   <si>
-    <t>['Pay Bills ', 'Withdraw cash']</t>
-  </si>
-  <si>
-    <t>['Cus_Nme', 'Amt_avail', 'Acc_type']['Bill_type', 'Max_limit']</t>
+    <t>['Pay Bills ']</t>
+  </si>
+  <si>
+    <t>{'Debit_pin', 'From_AcctNum', 'Amt_avail', 'Bill_type', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> apply for a loan</t>
@@ -74,7 +74,7 @@
     <t>['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr']['Loan_Amt', 'Cred_Score']</t>
+    <t>{'Debit_pin', 'From_AcctNum', 'Cus_Nme', 'To_AcctNum', 'Acc_num'}{'Loan_Amt', 'Loan_purp', 'Cred_Score'}</t>
   </si>
   <si>
     <t>Banker</t>
@@ -83,10 +83,10 @@
     <t xml:space="preserve"> request for check books</t>
   </si>
   <si>
-    <t>['Cheque Services', 'Verify PIN']</t>
-  </si>
-  <si>
-    <t>[]['Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_type']</t>
+    <t>['Cheque Services']</t>
+  </si>
+  <si>
+    <t>{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> restock sufficient cash</t>
@@ -95,16 +95,16 @@
     <t>['Restock cash', 'Limit Cash']</t>
   </si>
   <si>
-    <t>['Cus_Nme', 'Acc_type']['Cus_Nme', 'Acc_type']</t>
+    <t>{'Max_limit', 'Acc_type', 'Cus_Nme', 'Acc_num'}{'Debit_pin', 'Acc_type', 'Cus_Nme', 'Amt_deposit', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> limit the cash withdrawl</t>
   </si>
   <si>
-    <t>['Limit Cash', 'Withdraw cash']</t>
-  </si>
-  <si>
-    <t>['Cus_Nme', 'Acc_type']['Bill_type', 'Max_limit']</t>
+    <t>['Limit Cash']</t>
+  </si>
+  <si>
+    <t>{'Debit_pin', 'Acc_type', 'Cus_Nme', 'Amt_deposit', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> review all transactions</t>
@@ -113,7 +113,7 @@
     <t>['Review transactions', 'View Account ']</t>
   </si>
   <si>
-    <t>['Acc_num']['Acc_num', 'Amt_avail']</t>
+    <t>{'Acc_num'}{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
   </si>
   <si>
     <t xml:space="preserve"> review the credit history, apply for loans</t>
@@ -122,7 +122,7 @@
     <t>['Credit_check', 'Review transactions'],['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>['Loan_Amt', 'Cred_Score']['Acc_num'],['Loan_Amt', 'Amt_avail', 'Debit_pin', 'Amt_wdrl', 'Amt_trnsfr']['Loan_Amt', 'Cred_Score']</t>
+    <t>{'Loan_Amt', 'Loan_purp', 'Cred_Score'}{'Acc_num'},{'Debit_pin', 'From_AcctNum', 'Cus_Nme', 'To_AcctNum', 'Acc_num'}{'Loan_Amt', 'Loan_purp', 'Cred_Score'}</t>
   </si>
   <si>
     <t xml:space="preserve"> operate locker</t>
@@ -134,23 +134,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -165,26 +166,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,18 +487,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -649,9 +661,8 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added code to generate skeleton code for data elements
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
+++ b/SoftwareDesignUsingNLP/data/final_output_banking_2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10545" windowHeight="3585"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>User</t>
   </si>
@@ -38,7 +38,7 @@
     <t>['Verify PIN', 'Deposit Cheque']</t>
   </si>
   <si>
-    <t>{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}{'Debit_pin', 'Amt_avail', 'From_AcctNum', 'To_AcctNum', 'Acc_num'}</t>
+    <t>{'Cus_Nme', 'Acc_num', 'Loan_Amt', 'Cust_Addr'}{'Acc_num', 'Debit_pin', 'From_AcctNum', 'To_AcctNum', 'Amt_avail'}</t>
   </si>
   <si>
     <t xml:space="preserve"> withdraw cash</t>
@@ -47,7 +47,7 @@
     <t>['Withdraw cash', 'Verify PIN']</t>
   </si>
   <si>
-    <t>{'Debit_pin', 'Bill_type', 'Max_limit', 'Cus_Nme', 'Acc_num'}{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
+    <t>{'Cus_Nme', 'Acc_num', 'Debit_pin', 'Bill_type', 'Max_limit'}{'Cus_Nme', 'Acc_num', 'Loan_Amt', 'Cust_Addr'}</t>
   </si>
   <si>
     <t xml:space="preserve"> transfer money</t>
@@ -56,7 +56,7 @@
     <t>['Transfer Money', 'Verify PIN']</t>
   </si>
   <si>
-    <t>{'Amt_trnsfr', 'Amt_avail', 'Cus_Nme', 'To_AcctNum', 'From_AcctNum'}{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
+    <t>{'Cus_Nme', 'From_AcctNum', 'Amt_trnsfr', 'To_AcctNum', 'Amt_avail'}{'Cus_Nme', 'Acc_num', 'Loan_Amt', 'Cust_Addr'}</t>
   </si>
   <si>
     <t xml:space="preserve"> pay my utility bills</t>
@@ -65,7 +65,7 @@
     <t>['Pay Bills ']</t>
   </si>
   <si>
-    <t>{'Debit_pin', 'From_AcctNum', 'Amt_avail', 'Bill_type', 'Acc_num'}</t>
+    <t>{'Acc_num', 'Bill_type', 'Debit_pin', 'Amt_avail', 'From_AcctNum'}</t>
   </si>
   <si>
     <t xml:space="preserve"> apply for a loan</t>
@@ -74,7 +74,7 @@
     <t>['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>{'Debit_pin', 'From_AcctNum', 'Cus_Nme', 'To_AcctNum', 'Acc_num'}{'Loan_Amt', 'Loan_purp', 'Cred_Score'}</t>
+    <t>{'Cus_Nme', 'Acc_num', 'Debit_pin', 'To_AcctNum', 'From_AcctNum'}{'Loan_Amt', 'Loan_purp', 'Cred_Score'}</t>
   </si>
   <si>
     <t>Banker</t>
@@ -86,7 +86,7 @@
     <t>['Cheque Services']</t>
   </si>
   <si>
-    <t>{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
+    <t>{'Cus_Nme', 'Acc_num', 'Loan_Amt', 'Cust_Addr'}</t>
   </si>
   <si>
     <t xml:space="preserve"> restock sufficient cash</t>
@@ -95,7 +95,7 @@
     <t>['Restock cash', 'Limit Cash']</t>
   </si>
   <si>
-    <t>{'Max_limit', 'Acc_type', 'Cus_Nme', 'Acc_num'}{'Debit_pin', 'Acc_type', 'Cus_Nme', 'Amt_deposit', 'Acc_num'}</t>
+    <t>{'Cus_Nme', 'Acc_num', 'Acc_type', 'Max_limit'}{'Cus_Nme', 'Acc_num', 'Debit_pin', 'Acc_type', 'Amt_deposit'}</t>
   </si>
   <si>
     <t xml:space="preserve"> limit the cash withdrawl</t>
@@ -104,7 +104,7 @@
     <t>['Limit Cash']</t>
   </si>
   <si>
-    <t>{'Debit_pin', 'Acc_type', 'Cus_Nme', 'Amt_deposit', 'Acc_num'}</t>
+    <t>{'Cus_Nme', 'Acc_num', 'Debit_pin', 'Acc_type', 'Amt_deposit'}</t>
   </si>
   <si>
     <t xml:space="preserve"> review all transactions</t>
@@ -113,7 +113,7 @@
     <t>['Review transactions', 'View Account ']</t>
   </si>
   <si>
-    <t>{'Acc_num'}{'Cust_Addr', 'Loan_Amt', 'Cus_Nme', 'Acc_num'}</t>
+    <t>{'Acc_num'}{'Cus_Nme', 'Acc_num', 'Loan_Amt', 'Cust_Addr'}</t>
   </si>
   <si>
     <t xml:space="preserve"> review the credit history, apply for loans</t>
@@ -122,7 +122,7 @@
     <t>['Credit_check', 'Review transactions'],['Apply loan', 'Credit_check']</t>
   </si>
   <si>
-    <t>{'Loan_Amt', 'Loan_purp', 'Cred_Score'}{'Acc_num'},{'Debit_pin', 'From_AcctNum', 'Cus_Nme', 'To_AcctNum', 'Acc_num'}{'Loan_Amt', 'Loan_purp', 'Cred_Score'}</t>
+    <t>{'Loan_Amt', 'Loan_purp', 'Cred_Score'}{'Acc_num'},{'Cus_Nme', 'Acc_num', 'Debit_pin', 'To_AcctNum', 'From_AcctNum'}{'Loan_Amt', 'Loan_purp', 'Cred_Score'}</t>
   </si>
   <si>
     <t xml:space="preserve"> operate locker</t>
@@ -134,24 +134,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -166,40 +165,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -487,15 +472,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -661,8 +649,9 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
+      <c r="D12" t="s"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>